<commit_message>
Updation in custom order for both QA and STG
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>51540118</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>51540586</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="232">
+  <fills count="238">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1663,8 +1669,38 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="231">
+  <borders count="237">
     <border>
       <left/>
       <right/>
@@ -2545,11 +2581,32 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="124">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -2670,7 +2727,10 @@
     <xf applyBorder="true" applyFill="true" borderId="224" fillId="225" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="226" fillId="227" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="228" fillId="229" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="231" borderId="230" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="230" fillId="231" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="232" fillId="233" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="234" fillId="235" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="237" borderId="236" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3188,8 +3248,8 @@
       <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="115" t="s">
-        <v>149</v>
+      <c r="Q2" s="123" t="s">
+        <v>155</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="1" t="s">

</xml_diff>

<commit_message>
email update for request reroute
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="160">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -490,6 +490,18 @@
   </si>
   <si>
     <t>51540586</t>
+  </si>
+  <si>
+    <t>51540587</t>
+  </si>
+  <si>
+    <t>51540640</t>
+  </si>
+  <si>
+    <t>51540641</t>
+  </si>
+  <si>
+    <t>51540772</t>
   </si>
 </sst>
 </file>
@@ -512,7 +524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="238">
+  <fills count="252">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1699,8 +1711,78 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="237">
+  <borders count="251">
     <border>
       <left/>
       <right/>
@@ -2602,11 +2684,60 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="131">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -2730,7 +2861,14 @@
     <xf applyBorder="true" applyFill="true" borderId="230" fillId="231" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="232" fillId="233" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="234" fillId="235" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="237" borderId="236" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="236" fillId="237" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="238" fillId="239" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="240" fillId="241" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="242" fillId="243" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="244" fillId="245" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="246" fillId="247" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="248" fillId="249" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="251" borderId="250" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3248,8 +3386,8 @@
       <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="123" t="s">
-        <v>155</v>
+      <c r="Q2" s="128" t="s">
+        <v>157</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="1" t="s">
@@ -3332,8 +3470,8 @@
       <c r="P3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="118" t="s">
-        <v>150</v>
+      <c r="Q3" s="130" t="s">
+        <v>159</v>
       </c>
       <c r="R3" s="119" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
manage order BOL fixes.
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="161">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>51540772</t>
+  </si>
+  <si>
+    <t>51541535</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="252">
+  <fills count="254">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1781,8 +1784,18 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="251">
+  <borders count="253">
     <border>
       <left/>
       <right/>
@@ -2733,11 +2746,18 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="132">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -2868,7 +2888,8 @@
     <xf applyBorder="true" applyFill="true" borderId="244" fillId="245" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="246" fillId="247" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="248" fillId="249" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="251" borderId="250" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="250" fillId="251" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="253" borderId="252" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3470,8 +3491,8 @@
       <c r="P3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="130" t="s">
-        <v>159</v>
+      <c r="Q3" s="131" t="s">
+        <v>160</v>
       </c>
       <c r="R3" s="119" t="s">
         <v>152</v>

</xml_diff>

<commit_message>
updation of existing scripts
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_538.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="177">
   <si>
     <t>serviceLevel</t>
   </si>
@@ -535,6 +535,24 @@
   </si>
   <si>
     <t>51545897</t>
+  </si>
+  <si>
+    <t>51545935</t>
+  </si>
+  <si>
+    <t>08-21-2022</t>
+  </si>
+  <si>
+    <t>51545936</t>
+  </si>
+  <si>
+    <t>51545937</t>
+  </si>
+  <si>
+    <t>51545939</t>
+  </si>
+  <si>
+    <t>51545940</t>
   </si>
 </sst>
 </file>
@@ -557,7 +575,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="282">
+  <fills count="296">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1964,8 +1982,78 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="281">
+  <borders count="295">
     <border>
       <left/>
       <right/>
@@ -3021,11 +3109,60 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="153">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
@@ -3171,7 +3308,14 @@
     <xf applyBorder="true" applyFill="true" borderId="274" fillId="275" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="276" fillId="277" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="278" fillId="279" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="281" borderId="280" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="280" fillId="281" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="282" fillId="283" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="284" fillId="285" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="286" fillId="287" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="288" fillId="289" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="290" fillId="291" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="292" fillId="293" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="295" borderId="294" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3773,11 +3917,11 @@
       <c r="P3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="143" t="s">
-        <v>167</v>
-      </c>
-      <c r="R3" s="144" t="s">
-        <v>169</v>
+      <c r="Q3" s="152" t="s">
+        <v>176</v>
+      </c>
+      <c r="R3" s="149" t="s">
+        <v>173</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>31</v>
@@ -3804,8 +3948,8 @@
       <c r="AC3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="142" t="s">
-        <v>168</v>
+      <c r="AD3" s="147" t="s">
+        <v>172</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>56</v>
@@ -3859,8 +4003,8 @@
       <c r="P4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="145" t="s">
-        <v>170</v>
+      <c r="Q4" s="150" t="s">
+        <v>174</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="1" t="s">

</xml_diff>